<commit_message>
Libraries erstellt und eingebunden; Schema zeichnen begonnen
</commit_message>
<xml_diff>
--- a/Projektdokumente und Unterlagen/StücklisteSB.xlsx
+++ b/Projektdokumente und Unterlagen/StücklisteSB.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Position</t>
   </si>
@@ -53,126 +53,12 @@
     <t>Mouser</t>
   </si>
   <si>
-    <t xml:space="preserve">652-3362P-1-202LF </t>
-  </si>
-  <si>
-    <t>821-BZX55C2V0R0G</t>
-  </si>
-  <si>
     <t>Bauform</t>
   </si>
   <si>
-    <t>Flip-Flops 4bit w/Tri-St Out</t>
-  </si>
-  <si>
-    <t>BCD-to-7 segment latch/decoder/driver</t>
-  </si>
-  <si>
-    <t>Dual 4 bit Decade</t>
-  </si>
-  <si>
-    <t>Quad 2-Input AND gates</t>
-  </si>
-  <si>
-    <t>Schmitt-Trigger Inverter</t>
-  </si>
-  <si>
-    <t>7.62 mm Red Surface 7-Segment Display: CC</t>
-  </si>
-  <si>
-    <t>Abgewinkelt SPDT On-On</t>
-  </si>
-  <si>
-    <t>Drucktaster SMD</t>
-  </si>
-  <si>
-    <t>Buchse 4mm; 24A, 60VDC</t>
-  </si>
-  <si>
-    <t>Metallschichtwiderstand, THT; 1/4W; 1%;</t>
-  </si>
-  <si>
-    <t>BCD Decoder</t>
-  </si>
-  <si>
-    <t>D-Type Register</t>
-  </si>
-  <si>
-    <t>PDIP-14</t>
-  </si>
-  <si>
-    <t>PDIP-16</t>
-  </si>
-  <si>
-    <t>Zähler-IC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">595-SN74LS390N </t>
-  </si>
-  <si>
-    <t>THT Axial</t>
-  </si>
-  <si>
-    <t>AND Gatter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">595-SN74LS08N </t>
-  </si>
-  <si>
-    <t>Inverter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">595-SN74HC14N </t>
-  </si>
-  <si>
-    <t>7-Segment rot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">859-LTS-4801WC </t>
-  </si>
-  <si>
-    <t>Widerstand 270</t>
-  </si>
-  <si>
-    <t>Schiebeschalter</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>Drucktaster</t>
-  </si>
-  <si>
-    <t>1301.9320.24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OS102011MA1QN1 </t>
-  </si>
-  <si>
-    <t>Bananenbuchse rot</t>
-  </si>
-  <si>
-    <t>Banenenbuchse schwarz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Farnell </t>
-  </si>
-  <si>
-    <t>24.243.1</t>
-  </si>
-  <si>
-    <t>24.243.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">603-MFR-25FTE52-270R </t>
-  </si>
-  <si>
-    <t>Widerstand 47k</t>
-  </si>
-  <si>
-    <t>603-MFR-25FTE52-47K</t>
-  </si>
-  <si>
     <t>Total:</t>
   </si>
   <si>
@@ -191,16 +77,52 @@
     <t>8-Pin DFN</t>
   </si>
   <si>
-    <t>I2C Interface; 2.15V - 5.5V Supply; Accuracy of +/-2%RH and +/-0.2°C</t>
-  </si>
-  <si>
     <t xml:space="preserve">403-SHT30-DIS-F </t>
   </si>
   <si>
     <t>Protective Cover</t>
   </si>
   <si>
-    <t>Productive Cover for Temp. &amp; Hum. Sensor</t>
+    <t>Gyroskop</t>
+  </si>
+  <si>
+    <t>I3G4250DTR; X, Y, Z; 2.4V - 3.6V Supply; I2C/SPI Interface; programmable Range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">511-I3G4250DTR </t>
+  </si>
+  <si>
+    <t>LGA-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+SHT30-DIS-B2.5kS; I2C Interface; 2.15V - 5.5V Supply; Accuracy of +/-2%RH and +/-0.2°C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+SHT30-DIS-F2.5kS; Productive Cover for Temp. &amp; Hum. Sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">262-BMA423 </t>
+  </si>
+  <si>
+    <t>LGA-12</t>
+  </si>
+  <si>
+    <t>BMA423; X, Y, Z; 1.2V - 3.6V Supply; I2C/SPI Interface; programmable Range</t>
+  </si>
+  <si>
+    <t>Beschleunigungssensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">375-HC-SR04 </t>
+  </si>
+  <si>
+    <t>Ultraschall-Distanzmesser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+HC-SR04; PWM Out; 5V Supply</t>
   </si>
 </sst>
 </file>
@@ -836,7 +758,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,7 +786,7 @@
     </row>
     <row r="2" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="B2" s="44"/>
       <c r="C2" s="44"/>
@@ -883,10 +805,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>2</v>
@@ -904,22 +826,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
       <c r="B4" s="23" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="G4" s="12">
         <v>1</v>
@@ -932,22 +854,22 @@
         <v>2.89</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="66" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="8" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="G5" s="6">
         <v>1</v>
@@ -960,340 +882,214 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="66" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="G6" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6" s="36">
-        <v>1.43</v>
+        <v>7.18</v>
       </c>
       <c r="I6" s="37">
         <f t="shared" si="0"/>
-        <v>2.86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+        <v>7.18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="8" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="G7" s="6">
         <v>1</v>
       </c>
       <c r="H7" s="36">
-        <v>0.34799999999999998</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="I7" s="37">
         <f t="shared" si="0"/>
-        <v>0.34799999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G8" s="6">
         <v>1</v>
       </c>
       <c r="H8" s="36">
-        <v>1.4</v>
+        <v>5.44</v>
       </c>
       <c r="I8" s="37">
         <f t="shared" si="0"/>
-        <v>1.4</v>
+        <v>5.44</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
-      <c r="B9" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="6">
-        <v>1</v>
-      </c>
-      <c r="H9" s="36">
-        <v>0.60399999999999998</v>
-      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="36"/>
       <c r="I9" s="37">
         <f t="shared" si="0"/>
-        <v>0.60399999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
-      <c r="B10" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="6">
-        <v>1</v>
-      </c>
-      <c r="H10" s="36">
-        <v>0.55800000000000005</v>
-      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="36"/>
       <c r="I10" s="37">
         <f t="shared" si="0"/>
-        <v>0.55800000000000005</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
-      <c r="B11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="6">
-        <v>2</v>
-      </c>
-      <c r="H11" s="36">
-        <v>1.1599999999999999</v>
-      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="36"/>
       <c r="I11" s="37">
         <f t="shared" si="0"/>
-        <v>2.3199999999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
-      <c r="B12" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="6">
-        <v>14</v>
-      </c>
-      <c r="H12" s="36">
-        <v>0.11</v>
-      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="36"/>
       <c r="I12" s="37">
         <f t="shared" si="0"/>
-        <v>1.54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
-      <c r="B13" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="6">
-        <v>6</v>
-      </c>
-      <c r="H13" s="36">
-        <v>0.1</v>
-      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="36"/>
       <c r="I13" s="37">
         <f t="shared" si="0"/>
-        <v>0.60000000000000009</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
-      <c r="B14" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="6">
-        <v>2</v>
-      </c>
-      <c r="H14" s="36">
-        <v>0.34799999999999998</v>
-      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="36"/>
       <c r="I14" s="37">
         <f t="shared" si="0"/>
-        <v>0.69599999999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
-      <c r="B15" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="6">
-        <v>1</v>
-      </c>
-      <c r="H15" s="36">
-        <v>0.45500000000000002</v>
-      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="36"/>
       <c r="I15" s="37">
         <f t="shared" si="0"/>
-        <v>0.45500000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
-      <c r="B16" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="6">
-        <v>2</v>
-      </c>
-      <c r="H16" s="36">
-        <v>2.02</v>
-      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="36"/>
       <c r="I16" s="37">
         <f t="shared" si="0"/>
-        <v>4.04</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
-      <c r="B17" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" s="6">
-        <v>1</v>
-      </c>
-      <c r="H17" s="36">
-        <v>2.02</v>
-      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="36"/>
       <c r="I17" s="37">
         <f t="shared" si="0"/>
-        <v>2.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -1361,7 +1157,10 @@
       <c r="F22" s="5"/>
       <c r="G22" s="6"/>
       <c r="H22" s="37"/>
-      <c r="I22" s="37"/>
+      <c r="I22" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
@@ -1498,11 +1297,11 @@
       <c r="F32" s="21"/>
       <c r="G32" s="22"/>
       <c r="H32" s="39" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="I32" s="42">
         <f>SUM(I4:I31)</f>
-        <v>24.321000000000002</v>
+        <v>21.51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changend Designator K4 to Q1 and updated 'Stückliste'
</commit_message>
<xml_diff>
--- a/Projektdokumente und Unterlagen/StücklisteSB.xlsx
+++ b/Projektdokumente und Unterlagen/StücklisteSB.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>Position</t>
   </si>
@@ -137,7 +137,43 @@
     <t>I/O Erweiterer/Port Expander</t>
   </si>
   <si>
-    <t xml:space="preserve"> 604-APTD3216SRCPRV </t>
+    <t>APTD3216SRCPRV; SMD RED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED </t>
+  </si>
+  <si>
+    <t xml:space="preserve">863-NTR4501NT1G </t>
+  </si>
+  <si>
+    <t>SOT-23-3</t>
+  </si>
+  <si>
+    <t>NTR4501NT1G; 20V; 3.2A; N-Kanal</t>
+  </si>
+  <si>
+    <t>MOSFET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">604-APTD3216SRCPRV </t>
+  </si>
+  <si>
+    <t>K3</t>
+  </si>
+  <si>
+    <t>K5</t>
+  </si>
+  <si>
+    <t>K1</t>
+  </si>
+  <si>
+    <t>X5</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Q1</t>
   </si>
 </sst>
 </file>
@@ -772,8 +808,8 @@
   </sheetPr>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,7 +878,9 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="82.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
+      <c r="A4" s="23" t="s">
+        <v>42</v>
+      </c>
       <c r="B4" s="23" t="s">
         <v>14</v>
       </c>
@@ -870,7 +908,9 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="66" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="B5" s="8" t="s">
         <v>17</v>
       </c>
@@ -898,7 +938,9 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="66" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="B6" s="8" t="s">
         <v>18</v>
       </c>
@@ -926,7 +968,9 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+      <c r="A7" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="B7" s="8" t="s">
         <v>27</v>
       </c>
@@ -954,7 +998,9 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+      <c r="A8" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="B8" s="8" t="s">
         <v>29</v>
       </c>
@@ -982,7 +1028,9 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+      <c r="A9" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="B9" s="8" t="s">
         <v>34</v>
       </c>
@@ -1009,14 +1057,24 @@
         <v>1.23</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4"/>
+    <row r="10" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1206</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="F10" s="7" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G10" s="6">
         <v>1</v>
@@ -1029,18 +1087,34 @@
         <v>0.35599999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="36"/>
+    <row r="11" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1</v>
+      </c>
+      <c r="H11" s="36">
+        <v>0.33800000000000002</v>
+      </c>
       <c r="I11" s="37">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33800000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -1336,7 +1410,7 @@
       </c>
       <c r="I32" s="42">
         <f>SUM(I4:I31)</f>
-        <v>23.096000000000004</v>
+        <v>23.434000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>